<commit_message>
haurs historam (continuous data)
</commit_message>
<xml_diff>
--- a/Cardano-Historical-Data-July2021.xlsx
+++ b/Cardano-Historical-Data-July2021.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="Cardano Historical Data - Inves" sheetId="1" r:id="rId1"/>
     <sheet name="Perhitungan" sheetId="2" r:id="rId2"/>
-    <sheet name="Histogram" sheetId="3" r:id="rId3"/>
+    <sheet name="Histogram" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
   <si>
     <t>Date</t>
   </si>
@@ -256,6 +256,21 @@
   </si>
   <si>
     <t>Sumber Data</t>
+  </si>
+  <si>
+    <t>https://github.com/imzers/area-kecamatan-indonesia-2015</t>
+  </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>MEDIAN</t>
+  </si>
+  <si>
+    <t>Positive Skewed</t>
+  </si>
+  <si>
+    <t>Karena Mean lebih besar daripada Median</t>
   </si>
 </sst>
 </file>
@@ -785,7 +800,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -795,6 +810,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -803,6 +821,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -972,11 +997,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="118212864"/>
-        <c:axId val="125173760"/>
+        <c:axId val="124683392"/>
+        <c:axId val="124685312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="118212864"/>
+        <c:axId val="124683392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1000,14 +1025,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125173760"/>
+        <c:crossAx val="124685312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="125173760"/>
+        <c:axId val="124685312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1032,7 +1057,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118212864"/>
+        <c:crossAx val="124683392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1045,7 +1070,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1066,7 +1091,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Histogram</a:t>
+              <a:t>Histogram - 1304211061</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1168,11 +1193,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="125336960"/>
-        <c:axId val="125371904"/>
+        <c:axId val="162881536"/>
+        <c:axId val="162883456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="125336960"/>
+        <c:axId val="162881536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1196,14 +1221,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125371904"/>
+        <c:crossAx val="162883456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="125371904"/>
+        <c:axId val="162883456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1228,7 +1253,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="125336960"/>
+        <c:crossAx val="162881536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1241,7 +1266,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1286,16 +1311,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2356,16 +2381,16 @@
       <c r="A34" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2382,7 +2407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -2742,232 +2767,255 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:O24"/>
+  <dimension ref="B2:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:O17"/>
+      <selection activeCell="G17" sqref="G17:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="3:4" ht="15.75" thickBot="1"/>
-    <row r="3" spans="3:4">
+    <row r="2" spans="2:3" ht="15.75" thickBot="1"/>
+    <row r="3" spans="2:3">
+      <c r="B3" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="C3" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="3:4">
-      <c r="C4" s="3">
+    <row r="4" spans="2:3">
+      <c r="B4" s="3">
         <v>1.09521</v>
       </c>
-      <c r="D4" s="4">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:4">
-      <c r="C5" s="3">
+    <row r="5" spans="2:3">
+      <c r="B5" s="3">
         <v>1.13592</v>
       </c>
-      <c r="D5" s="4">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:4">
-      <c r="C6" s="3">
+    <row r="6" spans="2:3">
+      <c r="B6" s="3">
         <v>1.1766300000000001</v>
       </c>
-      <c r="D6" s="4">
+      <c r="C6" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:4">
-      <c r="C7" s="3">
+    <row r="7" spans="2:3">
+      <c r="B7" s="3">
         <v>1.2173400000000001</v>
       </c>
-      <c r="D7" s="4">
+      <c r="C7" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:4">
-      <c r="C8" s="3">
+    <row r="8" spans="2:3">
+      <c r="B8" s="3">
         <v>1.2580499999999999</v>
       </c>
-      <c r="D8" s="4">
+      <c r="C8" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="3:4">
-      <c r="C9" s="3">
+    <row r="9" spans="2:3">
+      <c r="B9" s="3">
         <v>1.2987600000000001</v>
       </c>
-      <c r="D9" s="4">
+      <c r="C9" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="3:4">
-      <c r="C10" s="3">
+    <row r="10" spans="2:3">
+      <c r="B10" s="3">
         <v>1.3394699999999999</v>
       </c>
-      <c r="D10" s="4">
+      <c r="C10" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="3:4">
-      <c r="C11" s="3">
+    <row r="11" spans="2:3">
+      <c r="B11" s="3">
         <v>1.38018</v>
       </c>
-      <c r="D11" s="4">
+      <c r="C11" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="3:4">
-      <c r="C12" s="3">
+    <row r="12" spans="2:3">
+      <c r="B12" s="3">
         <v>1.42089</v>
       </c>
-      <c r="D12" s="4">
+      <c r="C12" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="3:4">
-      <c r="C13" s="3">
+    <row r="13" spans="2:3">
+      <c r="B13" s="3">
         <v>1.4616</v>
       </c>
-      <c r="D13" s="4">
+      <c r="C13" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="3:4" ht="15.75" thickBot="1">
-      <c r="C14" s="5" t="s">
+    <row r="14" spans="2:3" ht="15.75" thickBot="1">
+      <c r="B14" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="5">
+      <c r="C14" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:15">
-      <c r="D17">
+    <row r="17" spans="3:14">
+      <c r="C17" s="11">
         <v>1</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="D17" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="G17" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-    </row>
-    <row r="18" spans="4:15">
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+    </row>
+    <row r="18" spans="3:14">
+      <c r="C18" s="11"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-    </row>
-    <row r="19" spans="4:15">
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-    </row>
-    <row r="20" spans="4:15">
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-    </row>
-    <row r="21" spans="4:15">
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-    </row>
-    <row r="22" spans="4:15">
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-    </row>
-    <row r="23" spans="4:15">
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-    </row>
-    <row r="24" spans="4:15">
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+    </row>
+    <row r="19" spans="3:14">
+      <c r="C19" s="11">
+        <v>2</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="G19" s="7">
+        <f>AVERAGE(Perhitungan!A2:A32)</f>
+        <v>1.2807774193548389</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+    </row>
+    <row r="20" spans="3:14">
+      <c r="C20" s="11"/>
+      <c r="D20" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="G20" s="7">
+        <f>MEDIAN(B4:B13)</f>
+        <v>1.278405</v>
+      </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+    </row>
+    <row r="21" spans="3:14">
+      <c r="C21" s="11">
+        <v>3</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="G21" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+    </row>
+    <row r="22" spans="3:14">
+      <c r="C22" s="11"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+    </row>
+    <row r="23" spans="3:14">
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+    </row>
+    <row r="24" spans="3:14">
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="H17:O17"/>
-    <mergeCell ref="H18:O18"/>
-    <mergeCell ref="H19:O19"/>
-    <mergeCell ref="H20:O20"/>
-    <mergeCell ref="H21:O21"/>
-    <mergeCell ref="H22:O22"/>
-    <mergeCell ref="H23:O23"/>
-    <mergeCell ref="H24:O24"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
+  <mergeCells count="9">
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="G21:L21"/>
+    <mergeCell ref="G17:L18"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data source tugas statistika minggu-4 TelU - 2021 - Dua kali kerja karena harus Histogram (Continuous Data)
</commit_message>
<xml_diff>
--- a/Cardano-Historical-Data-July2021.xlsx
+++ b/Cardano-Historical-Data-July2021.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="390" windowWidth="19875" windowHeight="7725" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="390" windowWidth="19875" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="Cardano Historical Data - Inves" sheetId="1" r:id="rId1"/>
@@ -258,9 +258,6 @@
     <t>Sumber Data</t>
   </si>
   <si>
-    <t>https://github.com/imzers/area-kecamatan-indonesia-2015</t>
-  </si>
-  <si>
     <t>MEAN</t>
   </si>
   <si>
@@ -271,6 +268,9 @@
   </si>
   <si>
     <t>Karena Mean lebih besar daripada Median</t>
+  </si>
+  <si>
+    <t>https://github.com/imzers/area-kecamatan-indonesia-2015/blob/main/Cardano-Historical-Data-July2021.xlsx</t>
   </si>
 </sst>
 </file>
@@ -800,7 +800,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -813,6 +813,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -823,11 +830,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -997,11 +1000,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="124683392"/>
-        <c:axId val="124685312"/>
+        <c:axId val="152929792"/>
+        <c:axId val="152838144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="124683392"/>
+        <c:axId val="152929792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1025,14 +1028,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124685312"/>
+        <c:crossAx val="152838144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="124685312"/>
+        <c:axId val="152838144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1057,7 +1060,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="124683392"/>
+        <c:crossAx val="152929792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1070,7 +1073,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1193,11 +1196,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="162881536"/>
-        <c:axId val="162883456"/>
+        <c:axId val="152875392"/>
+        <c:axId val="152877312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="162881536"/>
+        <c:axId val="152875392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1221,14 +1224,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162883456"/>
+        <c:crossAx val="152877312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="162883456"/>
+        <c:axId val="152877312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1253,7 +1256,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="162881536"/>
+        <c:crossAx val="152875392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1266,7 +1269,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1629,7 +1632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -2381,16 +2384,16 @@
       <c r="A34" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2407,7 +2410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -2769,8 +2772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2877,142 +2880,143 @@
       </c>
     </row>
     <row r="17" spans="3:14">
-      <c r="C17" s="11">
+      <c r="C17" s="8">
         <v>1</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="G17" s="9" t="s">
+      <c r="E17" s="13"/>
+      <c r="G17" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="3:14">
+      <c r="C18" s="8"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="3:14">
+      <c r="C19" s="8">
+        <v>2</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-    </row>
-    <row r="18" spans="3:14">
-      <c r="C18" s="11"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-    </row>
-    <row r="19" spans="3:14">
-      <c r="C19" s="11">
-        <v>2</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="10"/>
+      <c r="E19" s="13"/>
       <c r="G19" s="7">
         <f>AVERAGE(Perhitungan!A2:A32)</f>
         <v>1.2807774193548389</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
     </row>
     <row r="20" spans="3:14">
-      <c r="C20" s="11"/>
-      <c r="D20" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="10"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="13"/>
       <c r="G20" s="7">
         <f>MEDIAN(B4:B13)</f>
         <v>1.278405</v>
       </c>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
     </row>
     <row r="21" spans="3:14">
-      <c r="C21" s="11">
+      <c r="C21" s="8">
         <v>3</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="G21" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="10"/>
-      <c r="G21" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
     </row>
     <row r="22" spans="3:14">
-      <c r="C22" s="11"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
     </row>
     <row r="23" spans="3:14">
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
     </row>
     <row r="24" spans="3:14">
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="G17:L18"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D18:E18"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="G21:L21"/>
-    <mergeCell ref="G17:L18"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>